<commit_message>
All parsing table entries without errors
</commit_message>
<xml_diff>
--- a/Proj4ParsingTable.xlsx
+++ b/Proj4ParsingTable.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShizaQ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\Desktop\proj4-minic-SyntaxChecker-RecPredict-startup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA18B8D6-521F-4E94-84CE-C630D74A5A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2EBFB7-F35A-49FF-B326-73F766C4621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11664" yWindow="816" windowWidth="11652" windowHeight="8880" xr2:uid="{7808FBCE-421A-4DE4-A39A-0036AF15B73A}"/>
+    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7808FBCE-421A-4DE4-A39A-0036AF15B73A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -421,12 +420,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -575,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -587,9 +610,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,42 +959,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBE7964-6D3D-42CA-A021-A6338BB41787}">
   <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="52.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1053,12 +1088,12 @@
       <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3"/>
@@ -1071,14 +1106,14 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="20" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="20" t="s">
         <v>31</v>
       </c>
       <c r="R2" s="3"/>
@@ -1092,19 +1127,19 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AE2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="2"/>
@@ -1118,7 +1153,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="N3" s="2"/>
@@ -1134,17 +1169,17 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="13" t="s">
         <v>63</v>
       </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="10"/>
+      <c r="AE3" s="9"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="2"/>
@@ -1157,10 +1192,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="13" t="s">
         <v>66</v>
       </c>
       <c r="N4" s="2"/>
@@ -1180,19 +1215,19 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="2" t="s">
+      <c r="AC4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AD4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="10" t="s">
+      <c r="AE4" s="17" t="s">
         <v>65</v>
       </c>
       <c r="AF4" s="2"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="2"/>
@@ -1222,20 +1257,20 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="2" t="s">
+      <c r="AC5" s="13" t="s">
         <v>67</v>
       </c>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="10"/>
+      <c r="AE5" s="9"/>
       <c r="AF5" s="2"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="13" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="2"/>
@@ -1264,14 +1299,14 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="10"/>
+      <c r="AE6" s="9"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="2"/>
@@ -1302,16 +1337,16 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="10"/>
-      <c r="AF7" s="2" t="s">
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C8" s="2"/>
@@ -1342,13 +1377,13 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="2" t="s">
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="2"/>
@@ -1361,7 +1396,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="12" t="s">
         <v>73</v>
       </c>
       <c r="M9" s="2"/>
@@ -1370,7 +1405,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2" t="s">
+      <c r="S9" s="12" t="s">
         <v>73</v>
       </c>
       <c r="T9" s="2"/>
@@ -1382,19 +1417,19 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="2" t="s">
+      <c r="AC9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AD9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AE9" s="10" t="s">
+      <c r="AE9" s="18" t="s">
         <v>73</v>
       </c>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="2"/>
@@ -1408,11 +1443,11 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="P10" s="2"/>
@@ -1421,28 +1456,28 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="2" t="s">
+      <c r="V10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="13" t="s">
         <v>74</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="10"/>
+      <c r="AE10" s="9"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="2"/>
@@ -1455,18 +1490,18 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="13" t="s">
         <v>80</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="16" t="s">
         <v>83</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2" t="s">
+      <c r="S11" s="13" t="s">
         <v>81</v>
       </c>
       <c r="T11" s="2"/>
@@ -1478,19 +1513,19 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="2" t="s">
+      <c r="AC11" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AD11" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="AE11" s="10" t="s">
+      <c r="AE11" s="19" t="s">
         <v>79</v>
       </c>
       <c r="AF11" s="2"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="2"/>
@@ -1542,14 +1577,14 @@
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="10"/>
+      <c r="AE12" s="9"/>
       <c r="AF12" s="2"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="2"/>
@@ -1580,11 +1615,11 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
-      <c r="AE13" s="10"/>
+      <c r="AE13" s="9"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="2"/>
@@ -1593,7 +1628,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="12" t="s">
         <v>88</v>
       </c>
       <c r="I14" s="2"/>
@@ -1618,15 +1653,15 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
-      <c r="AE14" s="10"/>
+      <c r="AE14" s="9"/>
       <c r="AF14" s="2"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="2"/>
@@ -1656,35 +1691,35 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="10"/>
+      <c r="AE15" s="9"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="14" t="s">
         <v>92</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L16" s="2"/>
@@ -1704,39 +1739,39 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
-      <c r="AC16" s="2" t="s">
+      <c r="AC16" s="13" t="s">
         <v>92</v>
       </c>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="10"/>
+      <c r="AE16" s="9"/>
       <c r="AF16" s="2"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="13" t="s">
         <v>89</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="13" t="s">
         <v>89</v>
       </c>
       <c r="L17" s="2"/>
@@ -1756,15 +1791,15 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
-      <c r="AC17" s="2" t="s">
+      <c r="AC17" s="13" t="s">
         <v>89</v>
       </c>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="10"/>
+      <c r="AE17" s="9"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="2"/>
@@ -1793,15 +1828,15 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
-      <c r="AC18" s="2" t="s">
+      <c r="AC18" s="12" t="s">
         <v>95</v>
       </c>
       <c r="AD18" s="2"/>
-      <c r="AE18" s="10"/>
+      <c r="AE18" s="9"/>
       <c r="AF18" s="2"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="2"/>
@@ -1831,15 +1866,15 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
-      <c r="AC19" s="2" t="s">
+      <c r="AC19" s="13" t="s">
         <v>94</v>
       </c>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="10"/>
+      <c r="AE19" s="9"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="2"/>
@@ -1853,7 +1888,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="13" t="s">
         <v>97</v>
       </c>
       <c r="N20" s="2"/>
@@ -1869,17 +1904,17 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
-      <c r="AA20" s="2" t="s">
+      <c r="AA20" s="13" t="s">
         <v>96</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
-      <c r="AE20" s="10"/>
+      <c r="AE20" s="9"/>
       <c r="AF20" s="2"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="2"/>
@@ -1893,7 +1928,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="11" t="s">
         <v>98</v>
       </c>
       <c r="N21" s="2"/>
@@ -1911,15 +1946,15 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
-      <c r="AC21" s="2" t="s">
+      <c r="AC21" s="11" t="s">
         <v>98</v>
       </c>
       <c r="AD21" s="2"/>
-      <c r="AE21" s="10"/>
+      <c r="AE21" s="9"/>
       <c r="AF21" s="2"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="2"/>
@@ -1936,13 +1971,13 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2" t="s">
+      <c r="P22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="Q22" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="R22" s="11" t="s">
         <v>100</v>
       </c>
       <c r="S22" s="2"/>
@@ -1957,11 +1992,11 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
-      <c r="AE22" s="10"/>
+      <c r="AE22" s="9"/>
       <c r="AF22" s="2"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="2"/>
@@ -1969,7 +2004,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="13" t="s">
         <v>102</v>
       </c>
       <c r="H23" s="2"/>
@@ -1995,14 +2030,14 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
-      <c r="AE23" s="10"/>
+      <c r="AE23" s="9"/>
       <c r="AF23" s="2"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="13" t="s">
         <v>103</v>
       </c>
       <c r="C24" s="2"/>
@@ -2033,20 +2068,20 @@
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
-      <c r="AE24" s="10"/>
-      <c r="AF24" s="2" t="s">
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="13" t="s">
         <v>104</v>
       </c>
       <c r="G25" s="2"/>
@@ -2072,31 +2107,31 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AD25" s="2"/>
-      <c r="AE25" s="10"/>
+      <c r="AE25" s="9"/>
       <c r="AF25" s="2"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="13" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="13" t="s">
         <v>108</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="13" t="s">
         <v>109</v>
       </c>
       <c r="L26" s="2"/>
@@ -2116,15 +2151,15 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
-      <c r="AC26" s="2" t="s">
+      <c r="AC26" s="13" t="s">
         <v>105</v>
       </c>
       <c r="AD26" s="2"/>
-      <c r="AE26" s="10"/>
+      <c r="AE26" s="9"/>
       <c r="AF26" s="2"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="2"/>
@@ -2172,35 +2207,35 @@
         <v>111</v>
       </c>
       <c r="AD27" s="2"/>
-      <c r="AE27" s="10"/>
+      <c r="AE27" s="9"/>
       <c r="AF27" s="2"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="13" t="s">
         <v>111</v>
       </c>
       <c r="I28" s="2"/>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="13" t="s">
         <v>111</v>
       </c>
       <c r="L28" s="2"/>
@@ -2222,11 +2257,11 @@
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
-      <c r="AE28" s="10"/>
+      <c r="AE28" s="9"/>
       <c r="AF28" s="2"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B29" s="2"/>
@@ -2266,13 +2301,13 @@
       <c r="AD29" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AE29" s="10" t="s">
+      <c r="AE29" s="9" t="s">
         <v>116</v>
       </c>
       <c r="AF29" s="2"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="2"/>
@@ -2286,11 +2321,11 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2" t="s">
+      <c r="M30" s="13" t="s">
         <v>118</v>
       </c>
       <c r="N30" s="2"/>
-      <c r="O30" s="2" t="s">
+      <c r="O30" s="13" t="s">
         <v>118</v>
       </c>
       <c r="P30" s="2"/>
@@ -2299,29 +2334,29 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="2" t="s">
+      <c r="V30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="W30" s="2" t="s">
+      <c r="W30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="X30" s="2" t="s">
+      <c r="X30" s="13" t="s">
         <v>117</v>
       </c>
       <c r="Y30" s="2"/>
-      <c r="Z30" s="2" t="s">
+      <c r="Z30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="AA30" s="2" t="s">
+      <c r="AA30" s="13" t="s">
         <v>118</v>
       </c>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>
-      <c r="AE30" s="10"/>
+      <c r="AE30" s="9"/>
       <c r="AF30" s="2"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2360,11 +2395,11 @@
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
-      <c r="AE31" s="10"/>
+      <c r="AE31" s="9"/>
       <c r="AF31" s="2"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="2"/>
@@ -2378,10 +2413,10 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="N32" s="13" t="s">
         <v>120</v>
       </c>
       <c r="O32" s="2"/>
@@ -2395,20 +2430,20 @@
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
-      <c r="Z32" s="2" t="s">
+      <c r="Z32" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="AA32" s="2" t="s">
+      <c r="AA32" s="13" t="s">
         <v>121</v>
       </c>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
-      <c r="AE32" s="10"/>
+      <c r="AE32" s="9"/>
       <c r="AF32" s="2"/>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="2"/>
@@ -2420,7 +2455,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="12" t="s">
         <v>122</v>
       </c>
       <c r="L33" s="2"/>
@@ -2442,10 +2477,10 @@
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
-      <c r="AE33" s="10"/>
+      <c r="AE33" s="9"/>
       <c r="AF33" s="2"/>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2476,7 +2511,7 @@
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
-      <c r="AE34" s="10"/>
+      <c r="AE34" s="9"/>
       <c r="AF34" s="2"/>
     </row>
   </sheetData>

</xml_diff>